<commit_message>
added a piece I forgot to the parts list
</commit_message>
<xml_diff>
--- a/PCBs/Parts Needed for Subsytem PCBs.xlsx
+++ b/PCBs/Parts Needed for Subsytem PCBs.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d5d13c61c60eae0c/Documents/Space center/SubsystemPanelsDocumentationAndSourceCode/PCBs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_132D82C170E6E5F2A37BD6061C260243F1C6DDC5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5959A7C8-AE37-4F46-B344-1D53314BAC7B}"/>
+  <bookViews>
+    <workbookView xWindow="380" yWindow="380" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
   <si>
     <t>Subsystem PCB parts list</t>
   </si>
@@ -117,16 +126,18 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
       </rPr>
       <t>5V model.</t>
     </r>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve"> The following has the correct pinout</t>
     </r>
@@ -182,16 +193,18 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
       </rPr>
       <t xml:space="preserve">For speaker must be </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
       </rPr>
       <t>&gt;3W, 5W is safer</t>
     </r>
@@ -228,44 +241,68 @@
   </si>
   <si>
     <t>16 (2x pin headers)</t>
+  </si>
+  <si>
+    <t>For the Speaker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="28.0"/>
+      <sz val="28"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF1F1F1F"/>
       <name val="&quot;Google Sans&quot;"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -273,7 +310,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -283,7 +320,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -291,53 +334,47 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -527,456 +564,489 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="2" width="16.13"/>
-    <col customWidth="1" min="3" max="3" width="31.25"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.08984375" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="22.5">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="s">
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="22.5">
+      <c r="A22" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
+      <c r="D24" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="4">
-        <v>15.0</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="s">
+      <c r="B25" s="2">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="s">
+      <c r="D26" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="s">
+      <c r="D27" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="4">
-        <v>7.0</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="s">
+      <c r="B29" s="2">
+        <v>7</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="s">
+      <c r="D30" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="s">
+      <c r="D32" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="22.5">
+      <c r="A34" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E35" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="4" t="s">
+      <c r="D36" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E37" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -985,37 +1055,38 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D5"/>
-    <hyperlink r:id="rId2" ref="D6"/>
-    <hyperlink r:id="rId3" ref="D7"/>
-    <hyperlink r:id="rId4" ref="D8"/>
-    <hyperlink r:id="rId5" ref="D9"/>
-    <hyperlink r:id="rId6" ref="D10"/>
-    <hyperlink r:id="rId7" ref="E10"/>
-    <hyperlink r:id="rId8" ref="D11"/>
-    <hyperlink r:id="rId9" ref="D12"/>
-    <hyperlink r:id="rId10" ref="D13"/>
-    <hyperlink r:id="rId11" ref="D14"/>
-    <hyperlink r:id="rId12" ref="D15"/>
-    <hyperlink r:id="rId13" ref="D16"/>
-    <hyperlink r:id="rId14" ref="D17"/>
-    <hyperlink r:id="rId15" ref="D18"/>
-    <hyperlink r:id="rId16" ref="D19"/>
-    <hyperlink r:id="rId17" ref="E19"/>
-    <hyperlink r:id="rId18" ref="D20"/>
-    <hyperlink r:id="rId19" ref="D24"/>
-    <hyperlink r:id="rId20" ref="D25"/>
-    <hyperlink r:id="rId21" ref="D26"/>
-    <hyperlink r:id="rId22" ref="D27"/>
-    <hyperlink r:id="rId23" ref="D29"/>
-    <hyperlink r:id="rId24" ref="D30"/>
-    <hyperlink r:id="rId25" ref="D35"/>
-    <hyperlink r:id="rId26" ref="D36"/>
-    <hyperlink r:id="rId27" ref="E36"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D24" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D25" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D26" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D27" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D29" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D30" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D36" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D37" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E37" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D32" r:id="rId28" xr:uid="{189FD23C-E697-4065-83D8-C54F06687DEC}"/>
   </hyperlinks>
-  <drawing r:id="rId28"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>